<commit_message>
Prepare stats with new data
</commit_message>
<xml_diff>
--- a/06_Statistical_Preparation/KFactors_by_coupling/Lq_Lq.xlsx
+++ b/06_Statistical_Preparation/KFactors_by_coupling/Lq_Lq.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bibliotecas\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crisf\Downloads\Nueva carpeta (7)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4207D8C5-BE0F-44B0-96BF-2B586047A067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5666EE3C-287D-47A4-B26C-1F590BF80FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{936B0774-7D29-4A9D-A525-91C1BDE09DC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{936B0774-7D29-4A9D-A525-91C1BDE09DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,6 +75,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -474,128 +506,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85D8C1F-0C9C-4324-9C31-4CAB11EE0E07}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C1" s="2">
         <v>1250</v>
       </c>
-      <c r="C1" s="2">
+      <c r="D1" s="2">
         <v>1500</v>
       </c>
-      <c r="D1" s="2">
+      <c r="E1" s="2">
         <v>1750</v>
       </c>
-      <c r="E1" s="2">
+      <c r="F1" s="2">
         <v>2000</v>
       </c>
-      <c r="F1" s="2">
+      <c r="G1" s="2">
         <v>2250</v>
       </c>
-      <c r="G1" s="2">
+      <c r="H1">
         <v>2500</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>0.25</v>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.99170000000000003</v>
+        <v>1.0042418357438545</v>
       </c>
       <c r="C2" s="4">
-        <v>0.99399999999999999</v>
+        <v>0.9917217705832837</v>
       </c>
       <c r="D2" s="4">
-        <v>0.99409999999999998</v>
+        <v>0.99404185664420019</v>
       </c>
       <c r="E2" s="4">
-        <v>0.99119999999999997</v>
+        <v>0.99411372661032427</v>
       </c>
       <c r="F2" s="4">
-        <v>0.99099999999999999</v>
+        <v>0.99120568572452905</v>
       </c>
       <c r="G2" s="4">
-        <v>0.98619999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>0.5</v>
+        <v>0.99096321126788589</v>
+      </c>
+      <c r="H2">
+        <v>0.98615774919755805</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>0.99170000000000003</v>
+        <v>1.0078192875760208</v>
       </c>
       <c r="C3" s="4">
-        <v>0.99790000000000001</v>
+        <v>0.9917217705832837</v>
       </c>
       <c r="D3" s="4">
-        <v>0.99550000000000005</v>
+        <v>0.99785922168507657</v>
       </c>
       <c r="E3" s="4">
-        <v>0.99119999999999997</v>
+        <v>0.99551388678864872</v>
       </c>
       <c r="F3" s="4">
-        <v>0.99590000000000001</v>
+        <v>0.99120568572452905</v>
       </c>
       <c r="G3" s="4">
-        <v>0.99619999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>1</v>
+        <v>0.99593667782381001</v>
+      </c>
+      <c r="H3">
+        <v>0.99616950299651796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>0.99109999999999998</v>
+        <v>1.0052639648387591</v>
       </c>
       <c r="C4" s="4">
-        <v>0.99339999999999995</v>
+        <v>0.99112685650374965</v>
       </c>
       <c r="D4" s="4">
-        <v>0.99480000000000002</v>
+        <v>0.99343107823765997</v>
       </c>
       <c r="E4" s="4">
-        <v>0.99419999999999997</v>
+        <v>0.99481380669948638</v>
       </c>
       <c r="F4" s="4">
-        <v>0.98599999999999999</v>
+        <v>0.99421846896381338</v>
       </c>
       <c r="G4" s="4">
-        <v>1.0012000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>1.5</v>
+        <v>0.98598974471196177</v>
+      </c>
+      <c r="H4">
+        <v>1.0011753798959981</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>0.99409999999999998</v>
+        <v>1.0088414166709254</v>
       </c>
       <c r="C5" s="4">
-        <v>0.99939999999999996</v>
+        <v>0.99410142690141978</v>
       </c>
       <c r="D5" s="4">
-        <v>0.99339999999999995</v>
+        <v>0.99938616770142708</v>
       </c>
       <c r="E5" s="4">
-        <v>0.99119999999999997</v>
+        <v>0.99341364652116204</v>
       </c>
       <c r="F5" s="4">
-        <v>0.99839999999999995</v>
+        <v>0.99120568572452905</v>
       </c>
       <c r="G5" s="4">
-        <v>0.99619999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.99842341110177213</v>
+      </c>
+      <c r="H5">
+        <v>0.99616950299651796</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1.8</v>
       </c>
@@ -617,100 +664,116 @@
       <c r="G6" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>2</v>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>1.0081</v>
+        <v>1.0297950631164716</v>
       </c>
       <c r="C7" s="4">
-        <v>1.0109999999999999</v>
+        <v>1.0080819077704704</v>
       </c>
       <c r="D7" s="4">
-        <v>1.0108999999999999</v>
+        <v>1.0109909574256912</v>
       </c>
       <c r="E7" s="4">
-        <v>1.0063</v>
+        <v>1.0109156487502171</v>
       </c>
       <c r="F7" s="4">
-        <v>1.0022</v>
+        <v>1.0062696019209505</v>
       </c>
       <c r="G7" s="4">
-        <v>1.0012000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>2.5</v>
+        <v>1.0021535110187152</v>
+      </c>
+      <c r="H7">
+        <v>1.0011753798959981</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B8" s="4">
-        <v>1.0426</v>
+        <v>1.0635253232483262</v>
       </c>
       <c r="C8" s="4">
-        <v>1.0430999999999999</v>
+        <v>1.042586924383446</v>
       </c>
       <c r="D8" s="4">
-        <v>1.0333000000000001</v>
+        <v>1.0430568237690525</v>
       </c>
       <c r="E8" s="4">
-        <v>1.0304</v>
+        <v>1.0333182116034076</v>
       </c>
       <c r="F8" s="4">
-        <v>1.022</v>
+        <v>1.0303718678352249</v>
       </c>
       <c r="G8" s="4">
-        <v>1.0162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>3</v>
+        <v>1.0220473772424119</v>
+      </c>
+      <c r="H8">
+        <v>1.0161930105944379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B9" s="4">
-        <v>1.0975999999999999</v>
+        <v>1.1289415853222262</v>
       </c>
       <c r="C9" s="4">
-        <v>1.1003000000000001</v>
+        <v>1.0976164767403469</v>
       </c>
       <c r="D9" s="4">
-        <v>1.0871999999999999</v>
+        <v>1.1003172993821977</v>
       </c>
       <c r="E9" s="4">
-        <v>1.0755999999999999</v>
+        <v>1.0872243784688969</v>
       </c>
       <c r="F9" s="4">
-        <v>1.0581</v>
+        <v>1.0755636164244891</v>
       </c>
       <c r="G9" s="4">
-        <v>1.0511999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.0581050097728617</v>
+      </c>
+      <c r="H9">
+        <v>1.0512341488907977</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>3.5</v>
       </c>
       <c r="B10" s="4">
-        <v>1.1984999999999999</v>
+        <v>1.241886850309194</v>
       </c>
       <c r="C10" s="4">
-        <v>1.1900999999999999</v>
+        <v>1.1984544132213706</v>
       </c>
       <c r="D10" s="4">
-        <v>1.1739999999999999</v>
+        <v>1.1901017251436092</v>
       </c>
       <c r="E10" s="4">
-        <v>1.1478999999999999</v>
+        <v>1.1740343095250099</v>
       </c>
       <c r="F10" s="4">
-        <v>1.1228</v>
+        <v>1.1478704141673117</v>
       </c>
       <c r="G10" s="4">
-        <v>1.1012999999999999</v>
+        <v>1.1227600749998758</v>
+      </c>
+      <c r="H10">
+        <v>1.1012929178855977</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>